<commit_message>
Kanban con filtro listo
</commit_message>
<xml_diff>
--- a/src/main/webapp/content/files/plantilla.xlsx
+++ b/src/main/webapp/content/files/plantilla.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\LANIA\LOCAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DAC84D-4FD0-4317-AE36-B39451C7A435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D7770D-7BFF-4DAF-BDA8-A2923442D150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4425" yWindow="1575" windowWidth="19680" windowHeight="9585" xr2:uid="{B08329AC-7625-4388-9515-F2D5D066DBFF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{B08329AC-7625-4388-9515-F2D5D066DBFF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="CARGA INICIAL" sheetId="1" r:id="rId1"/>
+    <sheet name="Modificacion posterior" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="63">
   <si>
     <t>Id (Excel)</t>
   </si>
@@ -162,6 +163,69 @@
   </si>
   <si>
     <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Para despues</t>
+  </si>
+  <si>
+    <t>Por Asignar</t>
+  </si>
+  <si>
+    <t>Atributos Adicionales (etiquetas en gitlab)</t>
+  </si>
+  <si>
+    <t>Nombre 1</t>
+  </si>
+  <si>
+    <t>Descripción 2</t>
+  </si>
+  <si>
+    <t>Asignación (login) 4</t>
+  </si>
+  <si>
+    <t>iterasion 4</t>
+  </si>
+  <si>
+    <t>prioridad 5</t>
+  </si>
+  <si>
+    <t>Estatus 6</t>
+  </si>
+  <si>
+    <t>Puntos 7</t>
+  </si>
+  <si>
+    <t>Sin Iteracion</t>
+  </si>
+  <si>
+    <t>Historia de Usuario 1</t>
+  </si>
+  <si>
+    <t>Historia de Usuario 2</t>
+  </si>
+  <si>
+    <t>Historia de Usuario 3</t>
+  </si>
+  <si>
+    <t>Historia de Usuario 4</t>
+  </si>
+  <si>
+    <t>Historia de Usuario 5</t>
+  </si>
+  <si>
+    <t>Historia de Usuario 6</t>
+  </si>
+  <si>
+    <t>Historia de Usuario 7</t>
+  </si>
+  <si>
+    <t>Historia de Usuario 8</t>
+  </si>
+  <si>
+    <t>Historia de Usuario 9</t>
+  </si>
+  <si>
+    <t>Test Historia de Usuario 10</t>
   </si>
 </sst>
 </file>
@@ -239,24 +303,24 @@
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -574,10 +638,378 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB4AA57-102D-48C8-B5FF-57AEBDD42CE5}">
+  <dimension ref="A1:M12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" customWidth="1"/>
+    <col min="5" max="7" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8">
+        <v>30</v>
+      </c>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9">
+        <v>70</v>
+      </c>
+      <c r="I9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11">
+        <v>20</v>
+      </c>
+      <c r="I11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12">
+        <v>30</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="H1:M1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A280987D-1204-4FC2-B666-FAD981B2C4E0}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,69 +1019,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="4" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="6" t="s">
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -661,13 +1093,13 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="7">
         <v>45648</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>40</v>
       </c>
       <c r="G3" t="s">
@@ -699,13 +1131,13 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>45649</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>40</v>
       </c>
       <c r="G4" t="s">
@@ -737,13 +1169,13 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>45650</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="7" t="s">
         <v>34</v>
       </c>
       <c r="G5" t="s">
@@ -775,13 +1207,13 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>45651</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="7" t="s">
         <v>34</v>
       </c>
       <c r="G6" t="s">
@@ -813,13 +1245,13 @@
       <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <v>45652</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="7" t="s">
         <v>34</v>
       </c>
       <c r="G7" t="s">
@@ -851,13 +1283,13 @@
       <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="7">
         <v>45653</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="7" t="s">
         <v>34</v>
       </c>
       <c r="G8" t="s">
@@ -889,13 +1321,13 @@
       <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="7">
         <v>45654</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="7" t="s">
         <v>34</v>
       </c>
       <c r="G9" t="s">
@@ -927,13 +1359,13 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="7">
         <v>45655</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="7" t="s">
         <v>34</v>
       </c>
       <c r="G10" t="s">
@@ -965,13 +1397,13 @@
       <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="7">
         <v>45656</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="7" t="s">
         <v>34</v>
       </c>
       <c r="G11" t="s">
@@ -1003,13 +1435,13 @@
       <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <v>45657</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="7" t="s">
         <v>34</v>
       </c>
       <c r="G12" t="s">
@@ -1037,18 +1469,17 @@
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="K1:P1"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{2790CEE0-DB97-440A-B4B4-61F311AD535C}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{8FDFD541-DAD5-48E4-8ECB-159F6DA27D88}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{D932225F-AC51-4F81-A5D7-521A493E9B97}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{E7448D04-F270-47CD-A358-5C2BC66E771E}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{494FE20E-3120-4335-BCB7-5B959FF42BE4}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{B8F549DA-DC05-4AAD-9984-D4C8D5C926CB}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{F5F75338-A607-408A-ADEE-7EFF30CD13B3}"/>
-    <hyperlink ref="D10" r:id="rId8" xr:uid="{41167CF2-0A23-4561-A7BA-643700816D87}"/>
-    <hyperlink ref="D11" r:id="rId9" xr:uid="{C77D350C-E7DF-4867-83E6-6976B5F2D12E}"/>
-    <hyperlink ref="D12" r:id="rId10" xr:uid="{5A2BD66F-7E0B-478F-A0E3-FA4A6D7EF8EA}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{04EA6122-DB40-4E63-A909-83257FEB7C44}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{98A4E283-C33A-4F74-AB66-7239D46E2152}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{E98DC441-F0A2-4FA6-AECF-15319147DFD0}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{ED0B1DF3-7760-4E46-A74D-252A07FAEA61}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{A1994C21-7C27-4F03-BA79-CE8A0D401A13}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{C54AA88C-63BA-41BA-8EE5-CD7D1BA1EED8}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{E99F340E-47A0-4D40-8E6E-DF53A6359DED}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{9FD4D009-3C6B-4FD7-898E-7ABE38E13FBB}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{CF8DA912-82F3-4721-8C0B-F0D514FAA79B}"/>
+    <hyperlink ref="D12" r:id="rId10" xr:uid="{218302B8-1079-43C8-9FCF-8557C24820DB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>